<commit_message>
removed fastq_reformat subdirectory from fastqFilename path in modified sheets
</commit_message>
<xml_diff>
--- a/old_database/crypto/fastqFiles/fastq_314.xlsx
+++ b/old_database/crypto/fastqFiles/fastq_314.xlsx
@@ -46,79 +46,79 @@
     <t xml:space="preserve">Retrofitted_314</t>
   </si>
   <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_1_sequence_C1n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_1_sequence_C2n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_1_sequence_F1n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_1_sequence_F2n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_1_sequence_W2n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_2_sequence_C1p.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_2_sequence_C2p.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_2_sequence_F1p.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_2_sequence_F2p.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_2_sequence_W2p.fastq.gz</t>
+    <t xml:space="preserve">sequence/run_314_samples/s_1_sequence_C1n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_1_sequence_C2n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_1_sequence_F1n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_1_sequence_F2n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_1_sequence_W2n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_2_sequence_C1p.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_2_sequence_C2p.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_2_sequence_F1p.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_2_sequence_F2p.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_2_sequence_W2p.fastq.gz</t>
   </si>
   <si>
     <t xml:space="preserve">04.20.10</t>
   </si>
   <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_3_sequence_G1n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_3_sequence_G2n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_3_sequence_H1n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_3_sequence_H2n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_3_sequence_W4n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_4_sequence_G1p.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_4_sequence_G2p.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_4_sequence_H1p.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_4_sequence_H2p.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_4_sequence_W4p.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_5_sequence_W1n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_5_sequence_W1p.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_5_sequence_W3n.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_314_samples/fastq_reformat/s_5_sequence_W3p.fastq.gz</t>
+    <t xml:space="preserve">sequence/run_314_samples/s_3_sequence_G1n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_3_sequence_G2n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_3_sequence_H1n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_3_sequence_H2n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_3_sequence_W4n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_4_sequence_G1p.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_4_sequence_G2p.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_4_sequence_H1p.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_4_sequence_H2p.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_4_sequence_W4p.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_5_sequence_W1n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_5_sequence_W1p.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_5_sequence_W3n.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence/run_314_samples/s_5_sequence_W3p.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -238,13 +238,13 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="64.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="64.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>

</xml_diff>